<commit_message>
Updated 2016data.csv with more statistics
</commit_message>
<xml_diff>
--- a/data/Histograms/2016data.xlsx
+++ b/data/Histograms/2016data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YutongGu\Desktop\Powershell\DPSReportLog\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YutongGu\Desktop\Powershell\ReportSC\data\Histograms\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="99">
   <si>
     <t>THEFT-PETTY Theft Petty-Plain</t>
   </si>
@@ -295,6 +295,36 @@
   <si>
     <t>Top Incidents</t>
   </si>
+  <si>
+    <t>Traffic Collision Without Injury</t>
+  </si>
+  <si>
+    <t>Fire Alarm Malfunction</t>
+  </si>
+  <si>
+    <t>Outside USC Area</t>
+  </si>
+  <si>
+    <t>Traffic Collisions Without Injuries</t>
+  </si>
+  <si>
+    <t>The Lorenzo Apartments</t>
+  </si>
+  <si>
+    <t>Burglary-Residential</t>
+  </si>
+  <si>
+    <t>Welfare Check</t>
+  </si>
+  <si>
+    <t>General William Lyon University Center</t>
+  </si>
+  <si>
+    <t>University Gateway Apartments</t>
+  </si>
+  <si>
+    <t>Troy Hall</t>
+  </si>
 </sst>
 </file>
 
@@ -329,8 +359,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,11 +652,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="165060528"/>
-        <c:axId val="165065624"/>
+        <c:axId val="237693800"/>
+        <c:axId val="237691840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="165060528"/>
+        <c:axId val="237693800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -667,7 +699,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165065624"/>
+        <c:crossAx val="237691840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -675,7 +707,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165065624"/>
+        <c:axId val="237691840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -726,7 +758,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165060528"/>
+        <c:crossAx val="237693800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1047,11 +1079,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="165063272"/>
-        <c:axId val="165063664"/>
+        <c:axId val="237694192"/>
+        <c:axId val="237694584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="165063272"/>
+        <c:axId val="237694192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1094,7 +1126,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165063664"/>
+        <c:crossAx val="237694584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1102,7 +1134,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165063664"/>
+        <c:axId val="237694584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1153,7 +1185,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165063272"/>
+        <c:crossAx val="237694192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1474,11 +1506,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="426026992"/>
-        <c:axId val="426027384"/>
+        <c:axId val="237696152"/>
+        <c:axId val="238877904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="426026992"/>
+        <c:axId val="237696152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1521,7 +1553,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="426027384"/>
+        <c:crossAx val="238877904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1529,7 +1561,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="426027384"/>
+        <c:axId val="238877904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1580,7 +1612,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="426026992"/>
+        <c:crossAx val="237696152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1818,11 +1850,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="165067192"/>
-        <c:axId val="165064448"/>
+        <c:axId val="238881040"/>
+        <c:axId val="238880256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="165067192"/>
+        <c:axId val="238881040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1865,7 +1897,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165064448"/>
+        <c:crossAx val="238880256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1873,7 +1905,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165064448"/>
+        <c:axId val="238880256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1924,7 +1956,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165067192"/>
+        <c:crossAx val="238881040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2163,11 +2195,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="422187984"/>
-        <c:axId val="422190336"/>
+        <c:axId val="238884960"/>
+        <c:axId val="238882216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="422187984"/>
+        <c:axId val="238884960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2210,7 +2242,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422190336"/>
+        <c:crossAx val="238882216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2218,7 +2250,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="422190336"/>
+        <c:axId val="238882216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2269,7 +2301,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422187984"/>
+        <c:crossAx val="238884960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2508,11 +2540,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="422187592"/>
-        <c:axId val="422186416"/>
+        <c:axId val="238883000"/>
+        <c:axId val="238883392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="422187592"/>
+        <c:axId val="238883000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2555,7 +2587,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422186416"/>
+        <c:crossAx val="238883392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2563,7 +2595,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="422186416"/>
+        <c:axId val="238883392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2614,7 +2646,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422187592"/>
+        <c:crossAx val="238883000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2708,7 +2740,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2853,11 +2884,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="422186024"/>
-        <c:axId val="422188768"/>
+        <c:axId val="238883784"/>
+        <c:axId val="238884568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="422186024"/>
+        <c:axId val="238883784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2900,7 +2931,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422188768"/>
+        <c:crossAx val="238884568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2908,7 +2939,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="422188768"/>
+        <c:axId val="238884568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2959,7 +2990,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422186024"/>
+        <c:crossAx val="238883784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3048,7 +3079,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3193,11 +3223,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="422189552"/>
-        <c:axId val="422186808"/>
+        <c:axId val="238879864"/>
+        <c:axId val="238520272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="422189552"/>
+        <c:axId val="238879864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3240,7 +3270,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422186808"/>
+        <c:crossAx val="238520272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3248,7 +3278,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="422186808"/>
+        <c:axId val="238520272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3299,7 +3329,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422189552"/>
+        <c:crossAx val="238879864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3392,7 +3422,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3537,11 +3566,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="422190728"/>
-        <c:axId val="422183280"/>
+        <c:axId val="238519488"/>
+        <c:axId val="238519880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="422190728"/>
+        <c:axId val="238519488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3584,7 +3613,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422183280"/>
+        <c:crossAx val="238519880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3592,7 +3621,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="422183280"/>
+        <c:axId val="238519880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3643,7 +3672,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422190728"/>
+        <c:crossAx val="238519488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8734,8 +8763,8 @@
       <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
@@ -9556,17 +9585,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.21875" customWidth="1"/>
+    <col min="1" max="1" width="34.77734375" customWidth="1"/>
     <col min="4" max="4" width="18.77734375" customWidth="1"/>
     <col min="7" max="7" width="21.21875" customWidth="1"/>
+    <col min="10" max="10" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -9745,7 +9775,7 @@
         <v>1.0039740640033466E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -9756,7 +9786,7 @@
         <v>1.0039740640033466E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -9767,7 +9797,7 @@
         <v>9.8305793766994345E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>84</v>
       </c>
@@ -9778,7 +9808,7 @@
         <v>9.6214181133654052E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -9789,25 +9819,264 @@
         <v>9.6214181133654052E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>87</v>
       </c>
       <c r="D23" t="s">
         <v>86</v>
       </c>
+      <c r="G23" t="s">
+        <v>91</v>
+      </c>
+      <c r="J23" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>15</v>
       </c>
-      <c r="B24">
-        <v>100</v>
+      <c r="B24" s="1">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="D24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="G24" t="s">
+        <v>92</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="J24" t="s">
+        <v>4</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0.16700000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="1">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="J25" t="s">
+        <v>94</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0.111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="1">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="G26" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" s="1">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="J26" t="s">
+        <v>14</v>
+      </c>
+      <c r="K26" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="1">
+        <v>3.9E-2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="1">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="J27" t="s">
+        <v>95</v>
+      </c>
+      <c r="K27" s="1">
+        <v>6.9000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="1">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="1">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G28" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="1">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="J28" t="s">
+        <v>8</v>
+      </c>
+      <c r="K28" s="1">
+        <v>6.9000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" t="s">
+        <v>97</v>
+      </c>
+      <c r="G30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0.246</v>
+      </c>
+      <c r="G31" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0.216</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="D32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="G32" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" s="1">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="1">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="G33" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="1">
+        <v>7.8E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>95</v>
+      </c>
+      <c r="E34" s="1">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="G34" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="1">
+        <v>7.8E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="1">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="1">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G35" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" s="1">
+        <v>7.8E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>